<commit_message>
fffff andami kong naiba
</commit_message>
<xml_diff>
--- a/Messenger_Thesis_1._0/wwwroot/Book1.xlsx
+++ b/Messenger_Thesis_1._0/wwwroot/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian Radores\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC85807D-5DCA-4C0D-B85E-5E9D8BE04669}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E716625D-464B-4583-B407-F9B21FFE3BC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="1455" windowWidth="21600" windowHeight="11385" xr2:uid="{FC408E3A-AECD-4AC3-9BB1-211AD0A11940}"/>
+    <workbookView xWindow="1560" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{011B8471-E787-40DB-8422-1E8BE3A4347D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,33 +31,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
-  <si>
-    <t>Account name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>burat</t>
-  </si>
-  <si>
-    <t>keke</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>das</t>
-  </si>
-  <si>
-    <t>asd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+  <si>
+    <t>NAMe</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>Alberto Bugatsing</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>Areeya Mae</t>
+  </si>
+  <si>
+    <t>Jinkee Pacquiao</t>
+  </si>
+  <si>
+    <t>Shania Twain</t>
+  </si>
+  <si>
+    <t>Taylor Swift</t>
+  </si>
+  <si>
+    <t>Mitchel B.</t>
+  </si>
+  <si>
+    <t>Caloocan</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Pasig</t>
+  </si>
+  <si>
+    <t>Pasay</t>
+  </si>
+  <si>
+    <t>Mandaluyong</t>
   </si>
 </sst>
 </file>
@@ -408,14 +426,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C011ED-6885-4628-AD15-39FD7E1C7BB8}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B53FA5-9FBC-4AD4-87BE-AF199C199047}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -429,91 +450,69 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>20101</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20101</v>
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>20101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>20101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20101</v>
-      </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>20101</v>
+      <c r="A7" t="s">
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>20101</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>20101</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>